<commit_message>
Update MSSQL and some sample data
</commit_message>
<xml_diff>
--- a/data/DataGuide.xlsx
+++ b/data/DataGuide.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uithcm-my.sharepoint.com/personal/21520442_ms_uit_edu_vn/Documents/HKV/Internet &amp; Công nghệ web/FurnitureWebsite/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1012" documentId="11_F25DC773A252ABDACC10480FD91F48525BDE58F9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7D6A56D8-60F4-4BA3-A31B-A675DC698EDA}"/>
+  <xr:revisionPtr revIDLastSave="1026" documentId="11_F25DC773A252ABDACC10480FD91F48525BDE58F9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2BEAC499-6726-4864-879D-D81F4E72C980}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="13" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="968" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="952" uniqueCount="389">
   <si>
     <t>Procedure</t>
   </si>
@@ -215,9 +215,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t xml:space="preserve">enum('Shopping', 'Pending', 'Delivering', 'Complete', 'Cancelled')  </t>
-  </si>
-  <si>
     <t>date</t>
   </si>
   <si>
@@ -275,9 +272,6 @@
     <t>ValidDate</t>
   </si>
   <si>
-    <t>enum('Percentage', 'Value')</t>
-  </si>
-  <si>
     <t>Insert a voucher to VOUCHERS, auto ID</t>
   </si>
   <si>
@@ -1209,6 +1203,12 @@
   </si>
   <si>
     <t>decimal(10, 2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">varchar(25) in ('Shopping', 'Pending', 'Delivering', 'Complete', 'Cancelled')  </t>
+  </si>
+  <si>
+    <t>varchar(25) in enum('Percentage', 'Value')</t>
   </si>
 </sst>
 </file>
@@ -1945,10 +1945,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2214,10 +2210,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="B13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2374,24 +2370,24 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="47"/>
       <c r="B13" s="3" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D13" s="50"/>
       <c r="E13" s="56"/>
     </row>
-    <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="47"/>
       <c r="B14" s="3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D14" s="50"/>
       <c r="E14" s="56"/>
@@ -2399,10 +2395,10 @@
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="47"/>
       <c r="B15" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D15" s="50"/>
       <c r="E15" s="56"/>
@@ -2410,10 +2406,10 @@
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="47"/>
       <c r="B16" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D16" s="50"/>
       <c r="E16" s="56"/>
@@ -2421,10 +2417,10 @@
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="47"/>
       <c r="B17" s="3" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D17" s="50"/>
       <c r="E17" s="56"/>
@@ -2432,7 +2428,7 @@
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="47"/>
       <c r="B18" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>13</v>
@@ -2443,7 +2439,7 @@
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="47"/>
       <c r="B19" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>13</v>
@@ -2451,111 +2447,100 @@
       <c r="D19" s="50"/>
       <c r="E19" s="56"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="47"/>
-      <c r="B20" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C20" s="4" t="s">
+    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="48"/>
+      <c r="B20" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D20" s="50"/>
-      <c r="E20" s="56"/>
-    </row>
-    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="48"/>
-      <c r="B21" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D21" s="51"/>
-      <c r="E21" s="57"/>
-    </row>
-    <row r="22" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D20" s="51"/>
+      <c r="E20" s="57"/>
+    </row>
+    <row r="21" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="E21" s="22" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B22" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="C22" s="20" t="s">
-        <v>17</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="B22" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="44"/>
       <c r="D22" s="21" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="E22" s="22" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="B23" s="44" t="s">
-        <v>19</v>
-      </c>
-      <c r="C23" s="44"/>
+        <v>32</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>33</v>
+      </c>
       <c r="D23" s="21" t="s">
-        <v>29</v>
+        <v>65</v>
       </c>
       <c r="E23" s="22" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="18" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="D24" s="21" t="s">
-        <v>66</v>
+        <v>8</v>
+      </c>
+      <c r="D24" s="34" t="s">
+        <v>162</v>
       </c>
       <c r="E24" s="22" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="B25" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="C25" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="D25" s="34" t="s">
-        <v>164</v>
-      </c>
-      <c r="E25" s="22" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="14"/>
-      <c r="B26" s="27"/>
-      <c r="C26" s="28"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="14"/>
+      <c r="B25" s="27"/>
+      <c r="C25" s="28"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B22:C22"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A4:A11"/>
     <mergeCell ref="D4:D11"/>
     <mergeCell ref="E4:E11"/>
-    <mergeCell ref="D12:D21"/>
-    <mergeCell ref="E12:E21"/>
-    <mergeCell ref="A12:A21"/>
+    <mergeCell ref="D12:D20"/>
+    <mergeCell ref="E12:E20"/>
+    <mergeCell ref="A12:A20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2566,7 +2551,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2581,7 +2566,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A1" s="45" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B1" s="45"/>
       <c r="C1" s="45"/>
@@ -2614,10 +2599,10 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="46" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>8</v>
@@ -2626,13 +2611,13 @@
         <v>19</v>
       </c>
       <c r="E4" s="52" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="47"/>
       <c r="B5" s="3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>8</v>
@@ -2643,7 +2628,7 @@
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="47"/>
       <c r="B6" s="3" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>7</v>
@@ -2654,7 +2639,7 @@
     <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="58"/>
       <c r="B7" s="12" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C7" s="13" t="s">
         <v>13</v>
@@ -2664,19 +2649,19 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="46" t="s">
+        <v>223</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="49" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="52" t="s">
         <v>225</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="52" t="s">
-        <v>227</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>5</v>
@@ -2685,7 +2670,7 @@
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="47"/>
       <c r="B9" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>8</v>
@@ -2699,7 +2684,7 @@
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="47"/>
       <c r="B10" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>8</v>
@@ -2713,7 +2698,7 @@
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="47"/>
       <c r="B11" s="3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>8</v>
@@ -2727,7 +2712,7 @@
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="47"/>
       <c r="B12" s="3" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>7</v>
@@ -2741,7 +2726,7 @@
     <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="48"/>
       <c r="B13" s="7" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>13</v>
@@ -2751,10 +2736,10 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="46" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>8</v>
@@ -2763,13 +2748,13 @@
         <v>19</v>
       </c>
       <c r="E14" s="52" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="48"/>
       <c r="B15" s="7" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>8</v>
@@ -2779,74 +2764,74 @@
     </row>
     <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="16" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B16" s="71" t="s">
         <v>19</v>
       </c>
       <c r="C16" s="72"/>
       <c r="D16" s="33" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="16" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D17" s="33" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="18" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C18" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D18" s="21" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="61" t="s">
+        <v>235</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="59" t="s">
+        <v>236</v>
+      </c>
+      <c r="E19" s="55" t="s">
         <v>237</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D19" s="59" t="s">
-        <v>238</v>
-      </c>
-      <c r="E19" s="55" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="68"/>
       <c r="B20" s="7" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C20" s="8" t="s">
         <v>8</v>
@@ -2895,7 +2880,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A1" s="45" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B1" s="45"/>
       <c r="C1" s="45"/>
@@ -2928,10 +2913,10 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="46" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>8</v>
@@ -2940,13 +2925,13 @@
         <v>19</v>
       </c>
       <c r="E4" s="52" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="47"/>
       <c r="B5" s="3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>8</v>
@@ -2957,7 +2942,7 @@
     <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="47"/>
       <c r="B6" s="3" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>7</v>
@@ -2967,10 +2952,10 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="46" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>8</v>
@@ -2979,7 +2964,7 @@
         <v>19</v>
       </c>
       <c r="E7" s="52" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>5</v>
@@ -2988,7 +2973,7 @@
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="47"/>
       <c r="B8" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>8</v>
@@ -3002,7 +2987,7 @@
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="47"/>
       <c r="B9" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>8</v>
@@ -3016,7 +3001,7 @@
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="47"/>
       <c r="B10" s="3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>8</v>
@@ -3030,7 +3015,7 @@
     <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="47"/>
       <c r="B11" s="3" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>7</v>
@@ -3043,10 +3028,10 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="46" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>8</v>
@@ -3055,13 +3040,13 @@
         <v>19</v>
       </c>
       <c r="E12" s="52" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="48"/>
       <c r="B13" s="7" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>8</v>
@@ -3071,51 +3056,51 @@
     </row>
     <row r="14" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="16" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D14" s="33" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="16" t="s">
+        <v>247</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="33" t="s">
+        <v>248</v>
+      </c>
+      <c r="E15" s="11" t="s">
         <v>249</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" s="33" t="s">
-        <v>250</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="18" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B16" s="74" t="s">
         <v>19</v>
       </c>
       <c r="C16" s="75"/>
       <c r="D16" s="21" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
   </sheetData>
@@ -3156,7 +3141,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A1" s="45" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B1" s="45"/>
       <c r="C1" s="45"/>
@@ -3189,25 +3174,25 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="46" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="49" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="52" t="s">
         <v>257</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="52" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="58"/>
       <c r="B5" s="12" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>8</v>
@@ -3217,25 +3202,25 @@
     </row>
     <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="46" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="49" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="52" t="s">
         <v>261</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="52" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="47"/>
       <c r="B7" s="3" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>8</v>
@@ -3246,7 +3231,7 @@
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="47"/>
       <c r="B8" s="3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>8</v>
@@ -3257,7 +3242,7 @@
     <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="48"/>
       <c r="B9" s="7" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>8</v>
@@ -3267,10 +3252,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="46" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>8</v>
@@ -3279,13 +3264,13 @@
         <v>19</v>
       </c>
       <c r="E10" s="52" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="58"/>
       <c r="B11" s="12" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C11" s="13" t="s">
         <v>8</v>
@@ -3295,57 +3280,57 @@
     </row>
     <row r="12" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
+        <v>264</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>265</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="22" t="s">
         <v>266</v>
-      </c>
-      <c r="B12" s="19" t="s">
-        <v>267</v>
-      </c>
-      <c r="C12" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12" s="22" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="16" t="s">
+        <v>267</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>268</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="22" t="s">
         <v>269</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>270</v>
-      </c>
-      <c r="C13" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" s="22" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B14" s="44" t="s">
         <v>19</v>
       </c>
       <c r="C14" s="44"/>
       <c r="D14" s="21" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E14" s="22"/>
     </row>
     <row r="15" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="18" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C15" s="20" t="s">
         <v>8</v>
@@ -3354,15 +3339,15 @@
         <v>19</v>
       </c>
       <c r="E15" s="22" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="16" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C16" s="20" t="s">
         <v>8</v>
@@ -3371,7 +3356,7 @@
         <v>19</v>
       </c>
       <c r="E16" s="22" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -3383,6 +3368,10 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="D6:D9"/>
+    <mergeCell ref="E6:E9"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="D4:D5"/>
@@ -3390,10 +3379,6 @@
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="D10:D11"/>
     <mergeCell ref="E10:E11"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="D6:D9"/>
-    <mergeCell ref="E6:E9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3419,7 +3404,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A1" s="45" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B1" s="45"/>
       <c r="C1" s="45"/>
@@ -3452,10 +3437,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="46" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>8</v>
@@ -3464,13 +3449,13 @@
         <v>19</v>
       </c>
       <c r="E4" s="52" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="58"/>
       <c r="B5" s="12" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>8</v>
@@ -3480,10 +3465,10 @@
     </row>
     <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="46" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>8</v>
@@ -3492,13 +3477,13 @@
         <v>19</v>
       </c>
       <c r="E6" s="52" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="47"/>
       <c r="B7" s="3" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>8</v>
@@ -3509,7 +3494,7 @@
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="47"/>
       <c r="B8" s="3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>8</v>
@@ -3520,7 +3505,7 @@
     <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="48"/>
       <c r="B9" s="7" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>8</v>
@@ -3530,10 +3515,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="46" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>8</v>
@@ -3542,13 +3527,13 @@
         <v>19</v>
       </c>
       <c r="E10" s="52" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="58"/>
       <c r="B11" s="12" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C11" s="13" t="s">
         <v>8</v>
@@ -3558,10 +3543,10 @@
     </row>
     <row r="12" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C12" s="20" t="s">
         <v>8</v>
@@ -3570,15 +3555,15 @@
         <v>19</v>
       </c>
       <c r="E12" s="22" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="16" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C13" s="20" t="s">
         <v>8</v>
@@ -3587,28 +3572,28 @@
         <v>19</v>
       </c>
       <c r="E13" s="22" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B14" s="44" t="s">
         <v>19</v>
       </c>
       <c r="C14" s="44"/>
       <c r="D14" s="21" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E14" s="22"/>
     </row>
     <row r="15" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="18" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C15" s="20" t="s">
         <v>8</v>
@@ -3617,15 +3602,15 @@
         <v>19</v>
       </c>
       <c r="E15" s="22" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="16" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C16" s="20" t="s">
         <v>8</v>
@@ -3634,7 +3619,7 @@
         <v>19</v>
       </c>
       <c r="E16" s="22" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -3682,7 +3667,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A1" s="45" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B1" s="45"/>
       <c r="C1" s="45"/>
@@ -3715,10 +3700,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="46" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>8</v>
@@ -3727,13 +3712,13 @@
         <v>19</v>
       </c>
       <c r="E4" s="52" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="58"/>
       <c r="B5" s="12" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>8</v>
@@ -3743,10 +3728,10 @@
     </row>
     <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="46" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>8</v>
@@ -3755,13 +3740,13 @@
         <v>19</v>
       </c>
       <c r="E6" s="52" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="47"/>
       <c r="B7" s="3" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>8</v>
@@ -3772,7 +3757,7 @@
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="47"/>
       <c r="B8" s="3" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>8</v>
@@ -3783,7 +3768,7 @@
     <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="48"/>
       <c r="B9" s="7" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>8</v>
@@ -3793,10 +3778,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="46" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>8</v>
@@ -3805,13 +3790,13 @@
         <v>19</v>
       </c>
       <c r="E10" s="52" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="58"/>
       <c r="B11" s="12" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C11" s="13" t="s">
         <v>8</v>
@@ -3821,10 +3806,10 @@
     </row>
     <row r="12" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C12" s="20" t="s">
         <v>8</v>
@@ -3833,45 +3818,45 @@
         <v>19</v>
       </c>
       <c r="E12" s="22" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="16" t="s">
+        <v>307</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>308</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="22" t="s">
         <v>309</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>310</v>
-      </c>
-      <c r="C13" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" s="22" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B14" s="44" t="s">
         <v>19</v>
       </c>
       <c r="C14" s="44"/>
       <c r="D14" s="21" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E14" s="22"/>
     </row>
     <row r="15" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="18" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C15" s="20" t="s">
         <v>8</v>
@@ -3880,15 +3865,15 @@
         <v>19</v>
       </c>
       <c r="E15" s="22" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="16" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C16" s="20" t="s">
         <v>8</v>
@@ -3897,7 +3882,7 @@
         <v>19</v>
       </c>
       <c r="E16" s="22" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -3945,7 +3930,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A1" s="45" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B1" s="45"/>
       <c r="C1" s="45"/>
@@ -3978,19 +3963,19 @@
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="46" t="s">
+        <v>319</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="49" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="52" t="s">
         <v>321</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>295</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="52" t="s">
-        <v>323</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>5</v>
@@ -3999,7 +3984,7 @@
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="47"/>
       <c r="B5" s="3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>8</v>
@@ -4013,7 +3998,7 @@
     <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="47"/>
       <c r="B6" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>8</v>
@@ -4027,7 +4012,7 @@
     <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="58"/>
       <c r="B7" s="12" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C7" s="13" t="s">
         <v>8</v>
@@ -4037,10 +4022,10 @@
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="46" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>8</v>
@@ -4049,7 +4034,7 @@
         <v>19</v>
       </c>
       <c r="E8" s="52" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>5</v>
@@ -4058,7 +4043,7 @@
     <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="47"/>
       <c r="B9" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>8</v>
@@ -4072,7 +4057,7 @@
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="47"/>
       <c r="B10" s="3" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>8</v>
@@ -4086,7 +4071,7 @@
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="47"/>
       <c r="B11" s="3" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>8</v>
@@ -4100,7 +4085,7 @@
     <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="47"/>
       <c r="B12" s="3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>8</v>
@@ -4114,7 +4099,7 @@
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="47"/>
       <c r="B13" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>8</v>
@@ -4128,7 +4113,7 @@
     <row r="14" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="58"/>
       <c r="B14" s="12" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C14" s="13" t="s">
         <v>8</v>
@@ -4138,10 +4123,10 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="46" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>8</v>
@@ -4150,7 +4135,7 @@
         <v>19</v>
       </c>
       <c r="E15" s="52" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>5</v>
@@ -4159,7 +4144,7 @@
     <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="47"/>
       <c r="B16" s="3" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>8</v>
@@ -4173,7 +4158,7 @@
     <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="48"/>
       <c r="B17" s="7" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>8</v>
@@ -4181,49 +4166,49 @@
       <c r="D17" s="51"/>
       <c r="E17" s="54"/>
       <c r="I17" s="1" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="16" t="s">
+        <v>328</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="C18" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" s="11" t="s">
         <v>330</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>326</v>
-      </c>
-      <c r="C18" s="32" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" s="33" t="s">
-        <v>19</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="16" t="s">
+        <v>329</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>295</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" s="22" t="s">
         <v>331</v>
-      </c>
-      <c r="B19" s="19" t="s">
-        <v>297</v>
-      </c>
-      <c r="C19" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="D19" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="E19" s="22" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="16" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C20" s="20" t="s">
         <v>8</v>
@@ -4232,15 +4217,15 @@
         <v>19</v>
       </c>
       <c r="E20" s="22" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="16" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C21" s="32" t="s">
         <v>8</v>
@@ -4249,15 +4234,15 @@
         <v>19</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="16" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C22" s="20" t="s">
         <v>8</v>
@@ -4266,15 +4251,15 @@
         <v>19</v>
       </c>
       <c r="E22" s="22" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="16" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C23" s="20" t="s">
         <v>8</v>
@@ -4283,7 +4268,7 @@
         <v>19</v>
       </c>
       <c r="E23" s="22" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
   </sheetData>
@@ -4323,7 +4308,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A1" s="45" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B1" s="45"/>
       <c r="C1" s="45"/>
@@ -4356,10 +4341,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="46" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>8</v>
@@ -4368,13 +4353,13 @@
         <v>19</v>
       </c>
       <c r="E4" s="52" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="58"/>
       <c r="B5" s="12" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>8</v>
@@ -4384,10 +4369,10 @@
     </row>
     <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="46" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>8</v>
@@ -4396,13 +4381,13 @@
         <v>19</v>
       </c>
       <c r="E6" s="52" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="47"/>
       <c r="B7" s="3" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>8</v>
@@ -4413,7 +4398,7 @@
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="47"/>
       <c r="B8" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>8</v>
@@ -4424,7 +4409,7 @@
     <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="48"/>
       <c r="B9" s="7" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>8</v>
@@ -4434,10 +4419,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="46" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>8</v>
@@ -4446,13 +4431,13 @@
         <v>19</v>
       </c>
       <c r="E10" s="52" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="58"/>
       <c r="B11" s="12" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C11" s="13" t="s">
         <v>8</v>
@@ -4462,10 +4447,10 @@
     </row>
     <row r="12" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C12" s="20" t="s">
         <v>8</v>
@@ -4474,45 +4459,45 @@
         <v>19</v>
       </c>
       <c r="E12" s="22" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="16" t="s">
+        <v>353</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>354</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="22" t="s">
         <v>355</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>356</v>
-      </c>
-      <c r="C13" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" s="22" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B14" s="44" t="s">
         <v>19</v>
       </c>
       <c r="C14" s="44"/>
       <c r="D14" s="21" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E14" s="22"/>
     </row>
     <row r="15" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="18" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C15" s="20" t="s">
         <v>8</v>
@@ -4521,15 +4506,15 @@
         <v>19</v>
       </c>
       <c r="E15" s="22" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="16" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C16" s="20" t="s">
         <v>8</v>
@@ -4538,7 +4523,7 @@
         <v>19</v>
       </c>
       <c r="E16" s="22" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -4586,7 +4571,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A1" s="45" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B1" s="45"/>
       <c r="C1" s="45"/>
@@ -4619,10 +4604,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="46" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>8</v>
@@ -4631,13 +4616,13 @@
         <v>19</v>
       </c>
       <c r="E4" s="52" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="58"/>
       <c r="B5" s="12" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>8</v>
@@ -4647,10 +4632,10 @@
     </row>
     <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="46" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>8</v>
@@ -4659,13 +4644,13 @@
         <v>19</v>
       </c>
       <c r="E6" s="52" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="47"/>
       <c r="B7" s="3" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>8</v>
@@ -4676,7 +4661,7 @@
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="47"/>
       <c r="B8" s="3" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>8</v>
@@ -4687,7 +4672,7 @@
     <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="48"/>
       <c r="B9" s="7" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>8</v>
@@ -4697,10 +4682,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="46" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>8</v>
@@ -4709,13 +4694,13 @@
         <v>19</v>
       </c>
       <c r="E10" s="52" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="58"/>
       <c r="B11" s="12" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C11" s="13" t="s">
         <v>8</v>
@@ -4725,10 +4710,10 @@
     </row>
     <row r="12" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C12" s="20" t="s">
         <v>8</v>
@@ -4737,15 +4722,15 @@
         <v>19</v>
       </c>
       <c r="E12" s="22" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="16" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C13" s="20" t="s">
         <v>8</v>
@@ -4754,28 +4739,28 @@
         <v>19</v>
       </c>
       <c r="E13" s="22" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B14" s="44" t="s">
         <v>19</v>
       </c>
       <c r="C14" s="44"/>
       <c r="D14" s="21" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E14" s="22"/>
     </row>
     <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="18" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C15" s="20" t="s">
         <v>8</v>
@@ -4784,15 +4769,15 @@
         <v>19</v>
       </c>
       <c r="E15" s="22" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="16" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C16" s="20" t="s">
         <v>8</v>
@@ -4801,7 +4786,7 @@
         <v>19</v>
       </c>
       <c r="E16" s="22" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -4834,7 +4819,7 @@
   <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8:E11"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4849,7 +4834,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A1" s="45" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B1" s="45"/>
       <c r="C1" s="45"/>
@@ -4882,10 +4867,10 @@
     </row>
     <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="46" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>8</v>
@@ -4894,7 +4879,7 @@
         <v>19</v>
       </c>
       <c r="E4" s="52" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>5</v>
@@ -4903,10 +4888,10 @@
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="47"/>
       <c r="B5" s="3" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="D5" s="50"/>
       <c r="E5" s="53"/>
@@ -4914,7 +4899,7 @@
     <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="47"/>
       <c r="B6" s="3" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>8</v>
@@ -4928,7 +4913,7 @@
     <row r="7" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="58"/>
       <c r="B7" s="12" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C7" s="13" t="s">
         <v>8</v>
@@ -4938,10 +4923,10 @@
     </row>
     <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="46" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>8</v>
@@ -4950,16 +4935,16 @@
         <v>19</v>
       </c>
       <c r="E8" s="52" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="47"/>
       <c r="B9" s="3" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="D9" s="50"/>
       <c r="E9" s="53"/>
@@ -4967,7 +4952,7 @@
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="47"/>
       <c r="B10" s="3" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>8</v>
@@ -4978,7 +4963,7 @@
     <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="48"/>
       <c r="B11" s="7" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>8</v>
@@ -5009,10 +4994,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{196535D5-5947-4241-A508-57BB7B6E1270}">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5072,7 +5057,7 @@
         <v>19</v>
       </c>
       <c r="E4" s="55" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -5089,7 +5074,7 @@
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="47"/>
       <c r="B6" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C6" s="38" t="s">
         <v>11</v>
@@ -5100,10 +5085,10 @@
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="47"/>
       <c r="B7" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C7" s="38" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D7" s="60"/>
       <c r="E7" s="56"/>
@@ -5111,10 +5096,10 @@
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="47"/>
       <c r="B8" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C8" s="38" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D8" s="60"/>
       <c r="E8" s="56"/>
@@ -5122,10 +5107,10 @@
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="47"/>
       <c r="B9" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C9" s="38" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D9" s="60"/>
       <c r="E9" s="56"/>
@@ -5133,7 +5118,7 @@
     <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="58"/>
       <c r="B10" s="12" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C10" s="41" t="s">
         <v>8</v>
@@ -5155,16 +5140,16 @@
         <v>19</v>
       </c>
       <c r="E11" s="52" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="47"/>
       <c r="B12" s="3" t="s">
-        <v>24</v>
+        <v>172</v>
       </c>
       <c r="C12" s="38" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="D12" s="50"/>
       <c r="E12" s="53"/>
@@ -5172,10 +5157,10 @@
     <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="47"/>
       <c r="B13" s="3" t="s">
-        <v>174</v>
+        <v>42</v>
       </c>
       <c r="C13" s="38" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="D13" s="50"/>
       <c r="E13" s="53"/>
@@ -5183,10 +5168,10 @@
     <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="47"/>
       <c r="B14" s="3" t="s">
-        <v>42</v>
+        <v>163</v>
       </c>
       <c r="C14" s="38" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="D14" s="50"/>
       <c r="E14" s="53"/>
@@ -5194,10 +5179,10 @@
     <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="47"/>
       <c r="B15" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C15" s="38" t="s">
         <v>165</v>
-      </c>
-      <c r="C15" s="38" t="s">
-        <v>11</v>
       </c>
       <c r="D15" s="50"/>
       <c r="E15" s="53"/>
@@ -5224,97 +5209,103 @@
       <c r="D17" s="50"/>
       <c r="E17" s="53"/>
     </row>
-    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="47"/>
       <c r="B18" s="3" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="C18" s="38" t="s">
-        <v>171</v>
+        <v>57</v>
       </c>
       <c r="D18" s="50"/>
       <c r="E18" s="53"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="47"/>
-      <c r="B19" s="3" t="s">
+    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="48"/>
+      <c r="B19" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="C19" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="51"/>
+      <c r="E19" s="54"/>
+    </row>
+    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="C19" s="38" t="s">
-        <v>58</v>
-      </c>
-      <c r="D19" s="50"/>
-      <c r="E19" s="53"/>
-    </row>
-    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="48"/>
-      <c r="B20" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="C20" s="39" t="s">
-        <v>8</v>
-      </c>
-      <c r="D20" s="51"/>
-      <c r="E20" s="54"/>
-    </row>
-    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="16" t="s">
-        <v>44</v>
+        <v>177</v>
       </c>
       <c r="B21" s="31" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="C21" s="40" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="D21" s="33" t="s">
         <v>19</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="16" t="s">
-        <v>179</v>
-      </c>
-      <c r="B22" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" s="40" t="s">
-        <v>41</v>
-      </c>
-      <c r="D22" s="33" t="s">
-        <v>19</v>
-      </c>
-      <c r="E22" s="11" t="s">
-        <v>178</v>
+        <v>176</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="44"/>
+      <c r="D22" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="E22" s="22" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="B23" s="44" t="s">
-        <v>19</v>
-      </c>
-      <c r="C23" s="44"/>
+        <v>179</v>
+      </c>
+      <c r="B23" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="40" t="s">
+        <v>8</v>
+      </c>
       <c r="D23" s="21" t="s">
-        <v>49</v>
+        <v>180</v>
       </c>
       <c r="E23" s="22" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="18" t="s">
-        <v>181</v>
-      </c>
-      <c r="B24" s="31" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24" s="40" t="s">
-        <v>8</v>
+        <v>178</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" s="42" t="s">
+        <v>41</v>
       </c>
       <c r="D24" s="21" t="s">
         <v>182</v>
@@ -5325,69 +5316,52 @@
     </row>
     <row r="25" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="18" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>39</v>
+        <v>185</v>
       </c>
       <c r="C25" s="42" t="s">
         <v>41</v>
       </c>
       <c r="D25" s="21" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E25" s="22" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="18" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C26" s="42" t="s">
         <v>41</v>
       </c>
       <c r="D26" s="21" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E26" s="22" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="18" t="s">
         <v>189</v>
       </c>
-      <c r="B27" s="19" t="s">
-        <v>190</v>
-      </c>
-      <c r="C27" s="42" t="s">
-        <v>41</v>
-      </c>
-      <c r="D27" s="21" t="s">
-        <v>184</v>
-      </c>
-      <c r="E27" s="22" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="14"/>
-      <c r="B28" s="27"/>
-      <c r="C28" s="43"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="14"/>
+      <c r="B27" s="27"/>
+      <c r="C27" s="43"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="E11:E20"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="E11:E19"/>
     <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A11:A20"/>
-    <mergeCell ref="D11:D20"/>
+    <mergeCell ref="A11:A19"/>
+    <mergeCell ref="D11:D19"/>
     <mergeCell ref="A4:A10"/>
     <mergeCell ref="D4:D10"/>
     <mergeCell ref="E4:E10"/>
@@ -5398,10 +5372,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{064AD2A3-A134-48DE-87C5-78CF16E15D72}">
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5466,7 +5440,7 @@
     </row>
     <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="46" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>23</v>
@@ -5478,195 +5452,184 @@
         <v>19</v>
       </c>
       <c r="E5" s="52" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="47"/>
       <c r="B6" s="3" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>8</v>
+        <v>57</v>
       </c>
       <c r="D6" s="50"/>
       <c r="E6" s="53"/>
-    </row>
-    <row r="7" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="47"/>
       <c r="B7" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>58</v>
+        <v>8</v>
       </c>
       <c r="D7" s="50"/>
       <c r="E7" s="53"/>
-      <c r="L7" s="1" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="47"/>
       <c r="B8" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>8</v>
+        <v>55</v>
       </c>
       <c r="D8" s="50"/>
       <c r="E8" s="53"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="47"/>
-      <c r="B9" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D9" s="50"/>
-      <c r="E9" s="53"/>
-    </row>
-    <row r="10" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="48"/>
-      <c r="B10" s="7" t="s">
+    <row r="9" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="48"/>
+      <c r="B9" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C9" s="8" t="s">
+        <v>387</v>
+      </c>
+      <c r="D9" s="51"/>
+      <c r="E9" s="54"/>
+    </row>
+    <row r="10" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="44"/>
+      <c r="D11" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="E11" s="22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="18" t="s">
+        <v>195</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="42" t="s">
+        <v>196</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>197</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>191</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>387</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="E14" s="22" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="46" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D10" s="51"/>
-      <c r="E10" s="54"/>
-    </row>
-    <row r="11" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="B11" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="32" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="33" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="B12" s="44" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="44"/>
-      <c r="D12" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="E12" s="22" t="s">
+      <c r="D15" s="49" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="18" t="s">
-        <v>197</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="42" t="s">
-        <v>198</v>
-      </c>
-      <c r="D13" s="21" t="s">
-        <v>199</v>
-      </c>
-      <c r="E13" s="22" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="15" t="s">
-        <v>192</v>
-      </c>
-      <c r="B14" s="23" t="s">
-        <v>193</v>
-      </c>
-      <c r="C14" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="18" t="s">
-        <v>195</v>
-      </c>
-      <c r="B15" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="C15" s="20" t="s">
+      <c r="E15" s="52" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="48"/>
+      <c r="B16" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="D15" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="E15" s="22" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="46" t="s">
-        <v>67</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D16" s="49" t="s">
-        <v>65</v>
-      </c>
-      <c r="E16" s="52" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="48"/>
-      <c r="B17" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="D17" s="51"/>
-      <c r="E17" s="54"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
-      <c r="B18" s="27"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="54"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="14"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
     <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A5:A10"/>
-    <mergeCell ref="D5:D10"/>
-    <mergeCell ref="E5:E10"/>
-    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="A5:A9"/>
+    <mergeCell ref="D5:D9"/>
+    <mergeCell ref="E5:E9"/>
+    <mergeCell ref="B11:C11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5674,10 +5637,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC8DB291-0B00-48E3-AF0E-4BA557A5B82B}">
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5692,7 +5655,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A1" s="45" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B1" s="45"/>
       <c r="C1" s="45"/>
@@ -5725,7 +5688,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="61" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>3</v>
@@ -5737,16 +5700,16 @@
         <v>19</v>
       </c>
       <c r="E4" s="55" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="62"/>
       <c r="B5" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>77</v>
+        <v>388</v>
       </c>
       <c r="D5" s="60"/>
       <c r="E5" s="56"/>
@@ -5757,10 +5720,10 @@
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="62"/>
       <c r="B6" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>74</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>75</v>
       </c>
       <c r="D6" s="60"/>
       <c r="E6" s="56"/>
@@ -5768,10 +5731,10 @@
     <row r="7" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="62"/>
       <c r="B7" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D7" s="60"/>
       <c r="E7" s="56"/>
@@ -5781,7 +5744,7 @@
     </row>
     <row r="8" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="46" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>23</v>
@@ -5793,150 +5756,139 @@
         <v>19</v>
       </c>
       <c r="E8" s="52" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="47"/>
       <c r="B9" s="3" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="D9" s="50"/>
       <c r="E9" s="53"/>
-    </row>
-    <row r="10" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L9" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="47"/>
       <c r="B10" s="3" t="s">
-        <v>3</v>
+        <v>72</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>33</v>
+        <v>388</v>
       </c>
       <c r="D10" s="50"/>
       <c r="E10" s="53"/>
-      <c r="L10" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="47"/>
       <c r="B11" s="3" t="s">
         <v>73</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D11" s="50"/>
       <c r="E11" s="53"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="47"/>
-      <c r="B12" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C12" s="4" t="s">
+    <row r="12" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="48"/>
+      <c r="B12" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="D12" s="50"/>
-      <c r="E12" s="53"/>
-    </row>
-    <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="48"/>
-      <c r="B13" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="D13" s="51"/>
-      <c r="E13" s="54"/>
-    </row>
-    <row r="14" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="B14" s="31" t="s">
+      <c r="C12" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="51"/>
+      <c r="E12" s="54"/>
+    </row>
+    <row r="13" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="B13" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="32" t="s">
+      <c r="C13" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="33" t="s">
-        <v>19</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D13" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="B14" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="44"/>
+      <c r="D14" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="E14" s="22" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="B15" s="44" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="44"/>
+        <v>199</v>
+      </c>
+      <c r="B15" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="32" t="s">
+        <v>17</v>
+      </c>
       <c r="D15" s="21" t="s">
-        <v>85</v>
+        <v>200</v>
       </c>
       <c r="E15" s="22" t="s">
-        <v>86</v>
+        <v>201</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="18" t="s">
-        <v>201</v>
-      </c>
-      <c r="B16" s="31" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" s="32" t="s">
-        <v>17</v>
+        <v>85</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>33</v>
       </c>
       <c r="D16" s="21" t="s">
-        <v>202</v>
+        <v>111</v>
       </c>
       <c r="E16" s="22" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="B17" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="D17" s="21" t="s">
-        <v>113</v>
-      </c>
-      <c r="E17" s="22" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
-      <c r="B18" s="27"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="14"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="A4:A7"/>
     <mergeCell ref="D4:D7"/>
-    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B14:C14"/>
     <mergeCell ref="E4:E7"/>
     <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A8:A13"/>
-    <mergeCell ref="D8:D13"/>
-    <mergeCell ref="E8:E13"/>
+    <mergeCell ref="A8:A12"/>
+    <mergeCell ref="D8:D12"/>
+    <mergeCell ref="E8:E12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5944,10 +5896,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A034F745-31E9-4F50-BC6E-DD97F2A3C279}">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="B6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5962,7 +5914,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A1" s="45" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B1" s="45"/>
       <c r="C1" s="45"/>
@@ -5995,7 +5947,7 @@
     </row>
     <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>3</v>
@@ -6007,12 +5959,12 @@
         <v>19</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="46" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>23</v>
@@ -6024,46 +5976,50 @@
         <v>19</v>
       </c>
       <c r="E5" s="52" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="58"/>
+      <c r="B6" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="63"/>
+      <c r="E6" s="64"/>
+      <c r="L6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="22" t="s">
         <v>92</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="47"/>
-      <c r="B6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="50"/>
-      <c r="E6" s="53"/>
-    </row>
-    <row r="7" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="58"/>
-      <c r="B7" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" s="63"/>
-      <c r="E7" s="64"/>
-      <c r="L7" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="B8" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="20" t="s">
-        <v>17</v>
-      </c>
+      <c r="B8" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="44"/>
       <c r="D8" s="21" t="s">
-        <v>19</v>
+        <v>109</v>
       </c>
       <c r="E8" s="22" t="s">
         <v>94</v>
@@ -6071,67 +6027,52 @@
     </row>
     <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="B9" s="44" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="44"/>
+        <v>93</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>17</v>
+      </c>
       <c r="D9" s="21" t="s">
-        <v>111</v>
+        <v>202</v>
       </c>
       <c r="E9" s="22" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="18" t="s">
         <v>95</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>204</v>
+        <v>110</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="18" t="s">
-        <v>97</v>
-      </c>
-      <c r="B11" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="E11" s="22" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="27"/>
-      <c r="C12" s="28"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="14"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="E5:E7"/>
-    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="B8:C8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6139,10 +6080,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9E18967-B925-47B1-BE8F-A6126CB6B708}">
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="B7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6157,7 +6098,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A1" s="45" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B1" s="45"/>
       <c r="C1" s="45"/>
@@ -6190,7 +6131,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="61" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>3</v>
@@ -6202,23 +6143,23 @@
         <v>19</v>
       </c>
       <c r="E4" s="55" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="68"/>
       <c r="B5" s="7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D5" s="51"/>
       <c r="E5" s="57"/>
     </row>
     <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="65" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B6" s="27" t="s">
         <v>23</v>
@@ -6230,125 +6171,114 @@
         <v>19</v>
       </c>
       <c r="E6" s="67" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="47"/>
-      <c r="B7" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="50"/>
-      <c r="E7" s="53"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="58"/>
+      <c r="B7" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="63"/>
+      <c r="E7" s="64"/>
+    </row>
+    <row r="8" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="58"/>
       <c r="B8" s="12" t="s">
-        <v>3</v>
+        <v>100</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>33</v>
+        <v>101</v>
       </c>
       <c r="D8" s="63"/>
       <c r="E8" s="64"/>
-    </row>
-    <row r="9" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="58"/>
-      <c r="B9" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="D9" s="63"/>
-      <c r="E9" s="64"/>
-      <c r="L9" s="1" t="s">
+      <c r="L8" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="B10" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="20" t="s">
+      <c r="B10" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="44"/>
+      <c r="D10" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" s="22" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="18" t="s">
-        <v>109</v>
-      </c>
-      <c r="B11" s="44" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="44"/>
       <c r="D11" s="21" t="s">
-        <v>110</v>
+        <v>206</v>
       </c>
       <c r="E11" s="22" t="s">
-        <v>115</v>
+        <v>207</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="D12" s="21" t="s">
-        <v>208</v>
+        <v>114</v>
       </c>
       <c r="E12" s="22" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="18" t="s">
-        <v>207</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="21" t="s">
-        <v>116</v>
-      </c>
-      <c r="E13" s="22" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
-      <c r="B14" s="27"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="14"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B10:C10"/>
     <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="D6:D9"/>
-    <mergeCell ref="E6:E9"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="D6:D8"/>
+    <mergeCell ref="E6:E8"/>
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="E4:E5"/>
@@ -6359,10 +6289,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5759E5B-CF0F-4F7F-8744-A5B0DA70BAE3}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6377,7 +6307,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A1" s="45" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B1" s="45"/>
       <c r="C1" s="45"/>
@@ -6410,7 +6340,7 @@
     </row>
     <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B4" s="19" t="s">
         <v>3</v>
@@ -6422,12 +6352,12 @@
         <v>19</v>
       </c>
       <c r="E4" s="22" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="65" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B5" s="27" t="s">
         <v>23</v>
@@ -6439,111 +6369,100 @@
         <v>19</v>
       </c>
       <c r="E5" s="67" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="58"/>
+      <c r="B6" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="63"/>
+      <c r="E6" s="64"/>
+    </row>
+    <row r="7" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="22" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="47"/>
-      <c r="B6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="50"/>
-      <c r="E6" s="53"/>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="58"/>
-      <c r="B7" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" s="63"/>
-      <c r="E7" s="64"/>
-    </row>
-    <row r="8" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="B8" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="20" t="s">
-        <v>17</v>
-      </c>
+      <c r="B8" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="44"/>
       <c r="D8" s="21" t="s">
-        <v>19</v>
+        <v>124</v>
       </c>
       <c r="E8" s="22" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="s">
-        <v>125</v>
-      </c>
-      <c r="B9" s="44" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="44"/>
+        <v>208</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>17</v>
+      </c>
       <c r="D9" s="21" t="s">
+        <v>209</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="E9" s="22" t="s">
+      <c r="B10" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="21" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="18" t="s">
-        <v>210</v>
-      </c>
-      <c r="B10" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="21" t="s">
-        <v>211</v>
-      </c>
       <c r="E10" s="22" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="B11" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="21" t="s">
-        <v>129</v>
-      </c>
-      <c r="E11" s="22" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="27"/>
-      <c r="C12" s="28"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="14"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="E5:E7"/>
-    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="B8:C8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6551,10 +6470,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2612637-C604-420C-8C04-5550486ED857}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6569,7 +6488,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A1" s="45" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B1" s="45"/>
       <c r="C1" s="45"/>
@@ -6602,7 +6521,7 @@
     </row>
     <row r="4" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B4" s="19" t="s">
         <v>3</v>
@@ -6614,12 +6533,12 @@
         <v>19</v>
       </c>
       <c r="E4" s="22" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="65" t="s">
-        <v>134</v>
+      <c r="A5" s="61" t="s">
+        <v>132</v>
       </c>
       <c r="B5" s="27" t="s">
         <v>23</v>
@@ -6627,115 +6546,104 @@
       <c r="C5" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="66" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="67" t="s">
+      <c r="D5" s="59" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="55" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="68"/>
+      <c r="B6" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="73"/>
+      <c r="E6" s="57"/>
+    </row>
+    <row r="7" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="22" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="47"/>
-      <c r="B6" s="3" t="s">
+    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="B8" s="74" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="75"/>
+      <c r="D8" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="18" t="s">
+        <v>211</v>
+      </c>
+      <c r="B9" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="50"/>
-      <c r="E6" s="53"/>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="58"/>
-      <c r="B7" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" s="63"/>
-      <c r="E7" s="64"/>
-    </row>
-    <row r="8" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="18" t="s">
-        <v>136</v>
-      </c>
-      <c r="B8" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="20" t="s">
+      <c r="C9" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="22" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="18" t="s">
-        <v>139</v>
-      </c>
-      <c r="B9" s="44" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="44"/>
       <c r="D9" s="21" t="s">
-        <v>140</v>
+        <v>212</v>
       </c>
       <c r="E9" s="22" t="s">
-        <v>141</v>
+        <v>213</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="18" t="s">
-        <v>213</v>
+        <v>136</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>214</v>
+        <v>140</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="18" t="s">
-        <v>138</v>
-      </c>
-      <c r="B11" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="21" t="s">
-        <v>142</v>
-      </c>
-      <c r="E11" s="22" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="27"/>
-      <c r="C12" s="28"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
+        <v>141</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="14"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="E5:E7"/>
-    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="B8:C8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6761,7 +6669,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A1" s="45" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B1" s="45"/>
       <c r="C1" s="45"/>
@@ -6794,27 +6702,27 @@
     </row>
     <row r="4" spans="1:5" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="10" t="s">
         <v>145</v>
-      </c>
-      <c r="B4" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="C4" s="24" t="s">
-        <v>146</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="46" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>17</v>
@@ -6823,13 +6731,13 @@
         <v>19</v>
       </c>
       <c r="E5" s="52" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="48"/>
       <c r="B6" s="7" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>17</v>
@@ -6839,40 +6747,40 @@
     </row>
     <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="16" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B7" s="71" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="72"/>
       <c r="D7" s="33" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="61" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D8" s="59" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E8" s="55" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="68"/>
       <c r="B9" s="7" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>17</v>
@@ -6882,51 +6790,51 @@
     </row>
     <row r="10" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="18" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C10" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="B11" s="19" t="s">
         <v>157</v>
-      </c>
-      <c r="B11" s="19" t="s">
-        <v>159</v>
       </c>
       <c r="C11" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E11" s="22" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B12" s="69" t="s">
         <v>19</v>
       </c>
       <c r="C12" s="70"/>
       <c r="D12" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>